<commit_message>
Rename files & add IC for Historical MTOM runs & add format_newESP_files.r to read ESP text files to excel.
</commit_message>
<xml_diff>
--- a/Input Data/Observed_for_MTOM_IC.xlsx
+++ b/Input Data/Observed_for_MTOM_IC.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Reservoirs" sheetId="1" r:id="rId1"/>
     <sheet name="CoordinatedOps" sheetId="4" r:id="rId2"/>
-    <sheet name="FcstLocs" sheetId="3" r:id="rId3"/>
+    <sheet name="ForecastLocations" sheetId="3" r:id="rId3"/>
     <sheet name="InterveningFlow" sheetId="2" r:id="rId4"/>
     <sheet name="ICS" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -568,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S615"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -36867,7 +36867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished updating Initialization Rules.
</commit_message>
<xml_diff>
--- a/Input Data/Observed_for_MTOM_IC.xlsx
+++ b/Input Data/Observed_for_MTOM_IC.xlsx
@@ -207,25 +207,25 @@
     <t>HavasuToImperial:GainsPkrToImp.Local Inflow</t>
   </si>
   <si>
-    <t>PowellToMeadData.CarryoverVolume</t>
-  </si>
-  <si>
-    <t>PowellData.UpperElevBalBranch</t>
-  </si>
-  <si>
-    <t>PowellData.ReleaseTier</t>
-  </si>
-  <si>
-    <t>PowellData.TargetAnnualReleaseVolume</t>
-  </si>
-  <si>
     <t>* Prior to 2007 valuse are observed EOY values</t>
   </si>
   <si>
-    <t>PowellToMeadData.AugEOYPowellPEProjection_Input</t>
+    <t>MTOMRunType.CarryoverVolume_Input</t>
   </si>
   <si>
-    <t>PowellToMeadData.AugEOYMeadPEProjection_Input</t>
+    <t>MTOMRunType.AugEOYPowellPEProjection_Input</t>
+  </si>
+  <si>
+    <t>MTOMRunType.AugEOYMeadPEProjection_Input</t>
+  </si>
+  <si>
+    <t>MTOMRunType.ReleaseTier_Input</t>
+  </si>
+  <si>
+    <t>MTOMRunType.UpperElevBalBranch_Input</t>
+  </si>
+  <si>
+    <t>MTOMRunType.TargetAnnualReleaseVolume_Input</t>
   </si>
 </sst>
 </file>
@@ -36951,7 +36951,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36961,22 +36961,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -37894,7 +37894,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>